<commit_message>
Updated test cases of all
</commit_message>
<xml_diff>
--- a/src/test/java/adactinHotelApp/resources/TestData_AdactinHotelApp.xlsx
+++ b/src/test/java/adactinHotelApp/resources/TestData_AdactinHotelApp.xlsx
@@ -3,22 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A4A260F1-A00C-4A2E-B868-7166E9848255}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B89D6D39-526D-4CE9-AD08-18716825A138}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10725" yWindow="900" windowWidth="20790" windowHeight="11820" firstSheet="7" activeTab="7" xr2:uid="{5AC8F7C9-618F-4449-A92E-CFFD7E385ECD}"/>
+    <workbookView xWindow="10725" yWindow="900" windowWidth="20790" windowHeight="11820" firstSheet="2" activeTab="3" xr2:uid="{5AC8F7C9-618F-4449-A92E-CFFD7E385ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPositiveTest" sheetId="10" r:id="rId1"/>
     <sheet name="LoginNegativeTest" sheetId="2" r:id="rId2"/>
-    <sheet name="NewUserRegistration" sheetId="4" r:id="rId3"/>
+    <sheet name="RecoveryEmail" sheetId="14" r:id="rId3"/>
     <sheet name="ChangePassword" sheetId="13" r:id="rId4"/>
-    <sheet name="SearchHotelNegativeTest" sheetId="6" r:id="rId5"/>
-    <sheet name="SearchHotelPositiveTest" sheetId="11" r:id="rId6"/>
-    <sheet name="BookHotelPositiveTest" sheetId="12" r:id="rId7"/>
-    <sheet name="BookHotelNegativeTest" sheetId="9" r:id="rId8"/>
+    <sheet name="NewUserRegistration" sheetId="4" r:id="rId5"/>
+    <sheet name="SearchHotelNegativeTest" sheetId="6" r:id="rId6"/>
+    <sheet name="SearchHotelPositiveTest" sheetId="11" r:id="rId7"/>
+    <sheet name="BookHotelPositiveTest" sheetId="12" r:id="rId8"/>
+    <sheet name="BookHotelNegativeTest" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:G7"/>
+  <oleSize ref="A1:H11"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="53">
   <si>
     <t>UserName</t>
   </si>
@@ -174,7 +175,19 @@
     <t>Adactin20</t>
   </si>
   <si>
-    <t>Adactin2020</t>
+    <t>adactin2020@gmail.com</t>
+  </si>
+  <si>
+    <t>AdactinTrainee</t>
+  </si>
+  <si>
+    <t>adactin</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>adac</t>
   </si>
 </sst>
 </file>
@@ -553,7 +566,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,22 +598,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1D882F-76D8-4EF4-8383-374B7B97B850}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -611,7 +624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -619,10 +632,11 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -633,7 +647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -646,18 +660,138 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{8C4FDEF8-E792-4668-A1AD-60F750324261}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{4EBE41E9-97DB-48CE-9BCC-BE6A3F74FE17}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D718C13-5A4F-4227-842D-55DBB3D75289}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{367DB1EA-B43D-4FA7-A777-B7A4BEC1A17A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43BF7886-87D7-4F3B-A9AB-09065CF69860}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7CDF47D-5176-43F6-9A2A-CC185494F33C}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,67 +916,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43BF7886-87D7-4F3B-A9AB-09065CF69860}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{349F6FC1-BAEF-4A2B-A2E3-A4C844A2CC28}">
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,7 +996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -946,7 +1025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -975,7 +1054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1004,7 +1083,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -1034,7 +1113,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1064,7 +1143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1093,7 +1172,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1122,7 +1201,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1154,7 +1233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1192,12 +1271,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC0285F1-71FC-4F6D-B4E1-C93DDDF6969C}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,11 +1354,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B0D9F2-5866-471D-8943-5A1897847BA6}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
@@ -1292,7 +1371,7 @@
     <col min="19" max="19" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1348,7 +1427,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1409,12 +1488,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{301FC3F4-7F7E-42A7-B43E-AAC2E17DDDC2}">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1912,7 +1991,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="10" spans="1:18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1968,7 +2047,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -2018,7 +2097,7 @@
         <v>11</v>
       </c>
       <c r="Q11">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="R11">
         <v>123</v>

</xml_diff>